<commit_message>
3-add a bunch of data
</commit_message>
<xml_diff>
--- a/Resources/3-data.xlsx
+++ b/Resources/3-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>CO number</t>
   </si>
@@ -94,6 +94,30 @@
   </si>
   <si>
     <t>3013696384</t>
+  </si>
+  <si>
+    <t>3013696547</t>
+  </si>
+  <si>
+    <t>3013696548</t>
+  </si>
+  <si>
+    <t>3013696549</t>
+  </si>
+  <si>
+    <t>3013696550</t>
+  </si>
+  <si>
+    <t>3013696551</t>
+  </si>
+  <si>
+    <t>3013696552</t>
+  </si>
+  <si>
+    <t>3013696553</t>
+  </si>
+  <si>
+    <t>3013696554</t>
   </si>
 </sst>
 </file>
@@ -439,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,51 +582,91 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>17</v>
+      <c r="N4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3-update resource with working value
</commit_message>
<xml_diff>
--- a/Resources/3-data.xlsx
+++ b/Resources/3-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>CO number</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>3013696560</t>
+  </si>
+  <si>
+    <t>3013696566</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,6 +511,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
3-update with fresh data from M3
</commit_message>
<xml_diff>
--- a/Resources/3-data.xlsx
+++ b/Resources/3-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="13395" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="11475" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
   <si>
     <t>CO number</t>
   </si>
@@ -63,37 +63,46 @@
     <t xml:space="preserve">   Sched no</t>
   </si>
   <si>
-    <t>3013696551</t>
-  </si>
-  <si>
-    <t>3013696552</t>
-  </si>
-  <si>
-    <t>3013696553</t>
-  </si>
-  <si>
-    <t>3013696554</t>
-  </si>
-  <si>
-    <t>3013696555</t>
-  </si>
-  <si>
-    <t>3013696556</t>
-  </si>
-  <si>
-    <t>3013696557</t>
-  </si>
-  <si>
-    <t>3013696558</t>
-  </si>
-  <si>
-    <t>3013696559</t>
-  </si>
-  <si>
-    <t>3013696560</t>
-  </si>
-  <si>
-    <t>3013696566</t>
+    <t>TA5ACMFTWLC</t>
+  </si>
+  <si>
+    <t>101017</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>3013696592</t>
+  </si>
+  <si>
+    <t>3013696593</t>
+  </si>
+  <si>
+    <t>3013696594</t>
+  </si>
+  <si>
+    <t>3013696595</t>
+  </si>
+  <si>
+    <t>3013696596</t>
   </si>
 </sst>
 </file>
@@ -439,16 +448,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" style="1" customWidth="1"/>
@@ -513,57 +522,237 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
+      <c r="N6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2/3-update with fresh data
</commit_message>
<xml_diff>
--- a/Resources/3-data.xlsx
+++ b/Resources/3-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>CO number</t>
   </si>
@@ -88,12 +88,6 @@
   </si>
   <si>
     <t>001</t>
-  </si>
-  <si>
-    <t>3013696592</t>
-  </si>
-  <si>
-    <t>3013696593</t>
   </si>
   <si>
     <t>3013696594</t>
@@ -448,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD17"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,191 +561,97 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="N10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="3" t="s">
+      <c r="N11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>